<commit_message>
Upload Y4_B2526_General_&_Special_surgery_1_reference_data.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/reference_data/Y4_B2526_General_&_Special_surgery_1_reference_data.xlsx
+++ b/reference_data/Y4_B2526_General_&_Special_surgery_1_reference_data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="637">
   <si>
     <t>Student ID</t>
   </si>
@@ -1918,6 +1918,18 @@
   </si>
   <si>
     <t>B2F</t>
+  </si>
+  <si>
+    <t>تسنيم محمد انور</t>
+  </si>
+  <si>
+    <t>هاجر عماد حسين حسين</t>
+  </si>
+  <si>
+    <t>عمر محمد احمد على محمد حفناوى</t>
+  </si>
+  <si>
+    <t>محمد فتحى احمد الحسينى</t>
   </si>
 </sst>
 </file>
@@ -2303,10 +2315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E311"/>
+  <dimension ref="A1:E315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="D261" sqref="D261:D311"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="C316" sqref="C316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7605,6 +7617,74 @@
         <v>8</v>
       </c>
     </row>
+    <row r="312" spans="1:5">
+      <c r="A312" s="3">
+        <v>223003</v>
+      </c>
+      <c r="B312" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="C312" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D312" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E312" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="313" spans="1:5">
+      <c r="A313" s="3">
+        <v>223004</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C313" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D313" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E313" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="314" spans="1:5">
+      <c r="A314" s="3">
+        <v>223005</v>
+      </c>
+      <c r="B314" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="C314" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D314" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E314" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="315" spans="1:5">
+      <c r="A315" s="3">
+        <v>223006</v>
+      </c>
+      <c r="B315" s="3" t="s">
+        <v>636</v>
+      </c>
+      <c r="C315" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D315" s="3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E315" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update reference file: Y4_B2526_General_&_Special_surgery_1_reference_data.xlsx
</commit_message>
<xml_diff>
--- a/reference_data/Y4_B2526_General_&_Special_surgery_1_reference_data.xlsx
+++ b/reference_data/Y4_B2526_General_&_Special_surgery_1_reference_data.xlsx
@@ -1,12 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -25,12 +26,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <family val="2"/>
       <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b val="1"/>
@@ -70,19 +66,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -104,7 +91,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -469,7 +456,7 @@
   </sheetPr>
   <dimension ref="A1:E334"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -620,12 +607,12 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>190540</t>
+          <t>190796</t>
         </is>
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>ليان بنت خالد بن سعد المقذلى</t>
+          <t>اسيا ادريس ابراهيم ادريس</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -647,12 +634,12 @@
     <row r="7">
       <c r="A7" s="4" t="inlineStr">
         <is>
-          <t>190796</t>
+          <t>190801</t>
         </is>
       </c>
       <c r="B7" s="4" t="inlineStr">
         <is>
-          <t>اسيا ادريس ابراهيم ادريس</t>
+          <t>صالح سفيان محمد عثمان عابدون</t>
         </is>
       </c>
       <c r="C7" s="4" t="inlineStr">
@@ -674,12 +661,12 @@
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
         <is>
-          <t>190801</t>
+          <t>190803</t>
         </is>
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>صالح سفيان محمد عثمان عابدون</t>
+          <t>عبد الله كريم احمد الضمور</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -701,12 +688,12 @@
     <row r="9">
       <c r="A9" s="4" t="inlineStr">
         <is>
-          <t>190803</t>
+          <t>190807</t>
         </is>
       </c>
       <c r="B9" s="4" t="inlineStr">
         <is>
-          <t>عبد الله كريم احمد الضمور</t>
+          <t xml:space="preserve">ابراهيم عبد الجليل عبد الرحمن ابراهيم </t>
         </is>
       </c>
       <c r="C9" s="4" t="inlineStr">
@@ -728,12 +715,12 @@
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
         <is>
-          <t>190807</t>
+          <t>190846</t>
         </is>
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ابراهيم عبد الجليل عبد الرحمن ابراهيم </t>
+          <t>محمد ايهاب عبد الله حماد</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -755,12 +742,12 @@
     <row r="11">
       <c r="A11" s="4" t="inlineStr">
         <is>
-          <t>190846</t>
+          <t>190874</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
         <is>
-          <t>محمد ايهاب عبد الله حماد</t>
+          <t>محمد امين محمود حسن</t>
         </is>
       </c>
       <c r="C11" s="4" t="inlineStr">
@@ -782,12 +769,12 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>190874</t>
+          <t>190922</t>
         </is>
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>محمد امين محمود حسن</t>
+          <t>محمد عماد الدوس</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -809,12 +796,12 @@
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>190922</t>
+          <t>190929</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>محمد عماد الدوس</t>
+          <t>سلطان فازع على صغير</t>
         </is>
       </c>
       <c r="C13" s="4" t="inlineStr">
@@ -836,12 +823,12 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>190929</t>
+          <t>190968</t>
         </is>
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>سلطان فازع على صغير</t>
+          <t>احمد سليم بشير عجوز</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -863,12 +850,12 @@
     <row r="15">
       <c r="A15" s="4" t="inlineStr">
         <is>
-          <t>190968</t>
+          <t>190975</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
         <is>
-          <t>احمد سليم بشير عجوز</t>
+          <t>افنان صلاح عيسى حمد محمد</t>
         </is>
       </c>
       <c r="C15" s="4" t="inlineStr">
@@ -890,12 +877,12 @@
     <row r="16">
       <c r="A16" s="3" t="inlineStr">
         <is>
-          <t>190975</t>
+          <t>190981</t>
         </is>
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>افنان صلاح عيسى حمد محمد</t>
+          <t>عائشه موسى الراقى مهدى</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -917,12 +904,12 @@
     <row r="17">
       <c r="A17" s="4" t="inlineStr">
         <is>
-          <t>190981</t>
+          <t>191052</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
         <is>
-          <t>عائشه موسى الراقى مهدى</t>
+          <t>احمد رشاد حميد</t>
         </is>
       </c>
       <c r="C17" s="4" t="inlineStr">
@@ -944,12 +931,12 @@
     <row r="18">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>191052</t>
+          <t>191055</t>
         </is>
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>احمد رشاد حميد</t>
+          <t>بسام محمد سالم نويران</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -971,12 +958,12 @@
     <row r="19">
       <c r="A19" s="4" t="inlineStr">
         <is>
-          <t>191055</t>
+          <t>191061</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>بسام محمد سالم نويران</t>
+          <t xml:space="preserve"> Maya Naser Saleem Abubaker</t>
         </is>
       </c>
       <c r="C19" s="4" t="inlineStr">
@@ -998,12 +985,12 @@
     <row r="20">
       <c r="A20" s="3" t="inlineStr">
         <is>
-          <t>191061</t>
+          <t>191062</t>
         </is>
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Maya Naser Saleem Abubaker</t>
+          <t>احمد ابراهيم رمضان خضر</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1025,12 +1012,12 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>191062</t>
+          <t>191088</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>احمد ابراهيم رمضان خضر</t>
+          <t>عبد الرحمن عبود بشير محمد</t>
         </is>
       </c>
       <c r="C21" s="4" t="inlineStr">
@@ -1052,12 +1039,12 @@
     <row r="22">
       <c r="A22" s="3" t="inlineStr">
         <is>
-          <t>191088</t>
+          <t>191109</t>
         </is>
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>عبد الرحمن عبود بشير محمد</t>
+          <t>ريان بن احمد على العواجى</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1079,12 +1066,12 @@
     <row r="23">
       <c r="A23" s="4" t="inlineStr">
         <is>
-          <t>191109</t>
+          <t>191119</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>ريان بن احمد على العواجى</t>
+          <t xml:space="preserve">عمر بلال احمد الشدفان </t>
         </is>
       </c>
       <c r="C23" s="4" t="inlineStr">
@@ -1106,12 +1093,12 @@
     <row r="24">
       <c r="A24" s="3" t="inlineStr">
         <is>
-          <t>191119</t>
+          <t>191123</t>
         </is>
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">عمر بلال احمد الشدفان </t>
+          <t>حسين سعدأمين</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1133,12 +1120,12 @@
     <row r="25">
       <c r="A25" s="4" t="inlineStr">
         <is>
-          <t>191123</t>
+          <t>191125</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
         <is>
-          <t>حسين سعدأمين</t>
+          <t xml:space="preserve">احمد رائد محمد رفيق النتشه </t>
         </is>
       </c>
       <c r="C25" s="4" t="inlineStr">
@@ -1160,12 +1147,12 @@
     <row r="26">
       <c r="A26" s="3" t="inlineStr">
         <is>
-          <t>191125</t>
+          <t>191131</t>
         </is>
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">احمد رائد محمد رفيق النتشه </t>
+          <t xml:space="preserve">المثنى جاد عاطف  </t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1187,12 +1174,12 @@
     <row r="27">
       <c r="A27" s="4" t="inlineStr">
         <is>
-          <t>191131</t>
+          <t>191186</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">المثنى جاد عاطف  </t>
+          <t>ايمان ياسر محمد النونو</t>
         </is>
       </c>
       <c r="C27" s="4" t="inlineStr">
@@ -1214,12 +1201,12 @@
     <row r="28">
       <c r="A28" s="3" t="inlineStr">
         <is>
-          <t>191186</t>
+          <t>191258</t>
         </is>
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>ايمان ياسر محمد النونو</t>
+          <t xml:space="preserve">نايف محمد على الصغير الجلاب </t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1241,12 +1228,12 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>191258</t>
+          <t>191375</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">نايف محمد على الصغير الجلاب </t>
+          <t xml:space="preserve">هديل نصر الحريرى </t>
         </is>
       </c>
       <c r="C29" s="4" t="inlineStr">
@@ -1268,12 +1255,12 @@
     <row r="30">
       <c r="A30" s="3" t="inlineStr">
         <is>
-          <t>191375</t>
+          <t>191444</t>
         </is>
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">هديل نصر الحريرى </t>
+          <t>انس ناصر الشبراوى محمد محمد</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1295,12 +1282,12 @@
     <row r="31">
       <c r="A31" s="4" t="inlineStr">
         <is>
-          <t>191444</t>
+          <t>191478</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
         <is>
-          <t>انس ناصر الشبراوى محمد محمد</t>
+          <t>احمد عبد الرحمن محمد سامر النجار</t>
         </is>
       </c>
       <c r="C31" s="4" t="inlineStr">
@@ -1322,12 +1309,12 @@
     <row r="32">
       <c r="A32" s="3" t="inlineStr">
         <is>
-          <t>191478</t>
+          <t>191480</t>
         </is>
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>احمد عبد الرحمن محمد سامر النجار</t>
+          <t xml:space="preserve">محمد عمر سلامه الحراسيس </t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1349,12 +1336,12 @@
     <row r="33">
       <c r="A33" s="4" t="inlineStr">
         <is>
-          <t>191480</t>
+          <t>191502</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">محمد عمر سلامه الحراسيس </t>
+          <t>مرام حاتم عبد الله عباس</t>
         </is>
       </c>
       <c r="C33" s="4" t="inlineStr">
@@ -1376,12 +1363,12 @@
     <row r="34">
       <c r="A34" s="3" t="inlineStr">
         <is>
-          <t>191502</t>
+          <t>200003</t>
         </is>
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>مرام حاتم عبد الله عباس</t>
+          <t>ابراهيم جاد ابراهيم محمود</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1403,12 +1390,12 @@
     <row r="35">
       <c r="A35" s="4" t="inlineStr">
         <is>
-          <t>200003</t>
+          <t>200116</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>ابراهيم جاد ابراهيم محمود</t>
+          <t>اميره ابراهيم محمد</t>
         </is>
       </c>
       <c r="C35" s="4" t="inlineStr">
@@ -1430,12 +1417,12 @@
     <row r="36">
       <c r="A36" s="3" t="inlineStr">
         <is>
-          <t>200116</t>
+          <t>200163</t>
         </is>
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>اميره ابراهيم محمد</t>
+          <t>بسملة احمد عبدالمنعم خالد</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1457,12 +1444,12 @@
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>200163</t>
+          <t>200228</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
         <is>
-          <t>بسملة احمد عبدالمنعم خالد</t>
+          <t>رانا حسام رمضان محمد</t>
         </is>
       </c>
       <c r="C37" s="4" t="inlineStr">
@@ -1484,12 +1471,12 @@
     <row r="38">
       <c r="A38" s="3" t="inlineStr">
         <is>
-          <t>200228</t>
+          <t>200344</t>
         </is>
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>رانا حسام رمضان محمد</t>
+          <t>شريهان عبد الهادى السيد ابراهيم محمد</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1511,12 +1498,12 @@
     <row r="39">
       <c r="A39" s="4" t="inlineStr">
         <is>
-          <t>200344</t>
+          <t>200359</t>
         </is>
       </c>
       <c r="B39" s="4" t="inlineStr">
         <is>
-          <t>شريهان عبد الهادى السيد ابراهيم محمد</t>
+          <t>صلاح الدين عرفان صلاح عرفان محمد</t>
         </is>
       </c>
       <c r="C39" s="4" t="inlineStr">
@@ -1538,12 +1525,12 @@
     <row r="40">
       <c r="A40" s="3" t="inlineStr">
         <is>
-          <t>200359</t>
+          <t>200405</t>
         </is>
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>صلاح الدين عرفان صلاح عرفان محمد</t>
+          <t>عصام طه محمد صلاح الدين طه حسنين</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1565,12 +1552,12 @@
     <row r="41">
       <c r="A41" s="4" t="inlineStr">
         <is>
-          <t>200405</t>
+          <t>200423</t>
         </is>
       </c>
       <c r="B41" s="4" t="inlineStr">
         <is>
-          <t>عصام طه محمد صلاح الدين طه حسنين</t>
+          <t>عمر خالد احمد مختار هيكل</t>
         </is>
       </c>
       <c r="C41" s="4" t="inlineStr">
@@ -1592,12 +1579,12 @@
     <row r="42">
       <c r="A42" s="3" t="inlineStr">
         <is>
-          <t>200423</t>
+          <t>200468</t>
         </is>
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>عمر خالد احمد مختار هيكل</t>
+          <t>فريد مبروك حسين احمد ابوعامر</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1619,12 +1606,12 @@
     <row r="43">
       <c r="A43" s="4" t="inlineStr">
         <is>
-          <t>200468</t>
+          <t>200490</t>
         </is>
       </c>
       <c r="B43" s="4" t="inlineStr">
         <is>
-          <t>فريد مبروك حسين احمد ابوعامر</t>
+          <t>Kerlos Saber Kerlos Labib</t>
         </is>
       </c>
       <c r="C43" s="4" t="inlineStr">
@@ -1646,12 +1633,12 @@
     <row r="44">
       <c r="A44" s="3" t="inlineStr">
         <is>
-          <t>200490</t>
+          <t>200491</t>
         </is>
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>Kerlos Saber Kerlos Labib</t>
+          <t>كيرلس صفوت واصفي سوريال</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1673,12 +1660,12 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>200491</t>
+          <t>200628</t>
         </is>
       </c>
       <c r="B45" s="4" t="inlineStr">
         <is>
-          <t>كيرلس صفوت واصفي سوريال</t>
+          <t>منار سعيد حسن حسن الديب</t>
         </is>
       </c>
       <c r="C45" s="4" t="inlineStr">
@@ -1700,12 +1687,12 @@
     <row r="46">
       <c r="A46" s="3" t="inlineStr">
         <is>
-          <t>200628</t>
+          <t>200708</t>
         </is>
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>منار سعيد حسن حسن الديب</t>
+          <t>نورهان مجدى على احمد ابو شعير</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1727,12 +1714,12 @@
     <row r="47">
       <c r="A47" s="4" t="inlineStr">
         <is>
-          <t>200708</t>
+          <t>200727</t>
         </is>
       </c>
       <c r="B47" s="4" t="inlineStr">
         <is>
-          <t>نورهان مجدى على احمد ابو شعير</t>
+          <t>هبه محمد محمود عبدالظاهر احمد</t>
         </is>
       </c>
       <c r="C47" s="4" t="inlineStr">
@@ -1754,12 +1741,12 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>200727</t>
+          <t>200742</t>
         </is>
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>هبه محمد محمود عبدالظاهر احمد</t>
+          <t>ياسمين رفيق عبده التابعى يحيى</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1781,12 +1768,12 @@
     <row r="49">
       <c r="A49" s="4" t="inlineStr">
         <is>
-          <t>200742</t>
+          <t>200744</t>
         </is>
       </c>
       <c r="B49" s="4" t="inlineStr">
         <is>
-          <t>ياسمين رفيق عبده التابعى يحيى</t>
+          <t xml:space="preserve"> ياسمين مصطفى ابراهيم على السيسى</t>
         </is>
       </c>
       <c r="C49" s="4" t="inlineStr">
@@ -1808,12 +1795,12 @@
     <row r="50">
       <c r="A50" s="3" t="inlineStr">
         <is>
-          <t>200744</t>
+          <t>200785</t>
         </is>
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> ياسمين مصطفى ابراهيم على السيسى</t>
+          <t>ساره عبد الله احمد دانعي</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -1835,12 +1822,12 @@
     <row r="51">
       <c r="A51" s="4" t="inlineStr">
         <is>
-          <t>200785</t>
+          <t>200792</t>
         </is>
       </c>
       <c r="B51" s="4" t="inlineStr">
         <is>
-          <t>ساره عبد الله احمد دانعي</t>
+          <t>روان زكريا صالح</t>
         </is>
       </c>
       <c r="C51" s="4" t="inlineStr">
@@ -1862,12 +1849,12 @@
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
         <is>
-          <t>200792</t>
+          <t>200804</t>
         </is>
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>روان زكريا صالح</t>
+          <t>Asma Haji Osman Omer</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -1889,12 +1876,12 @@
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>200804</t>
+          <t>200824</t>
         </is>
       </c>
       <c r="B53" s="4" t="inlineStr">
         <is>
-          <t>Asma Haji Osman Omer</t>
+          <t>محمد نظام محمد القرا</t>
         </is>
       </c>
       <c r="C53" s="4" t="inlineStr">
@@ -1916,12 +1903,12 @@
     <row r="54">
       <c r="A54" s="3" t="inlineStr">
         <is>
-          <t>200824</t>
+          <t>200850</t>
         </is>
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>محمد نظام محمد القرا</t>
+          <t>دانيه مصطفى سالم يوسف</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -1931,7 +1918,7 @@
       </c>
       <c r="D54" s="3" t="inlineStr">
         <is>
-          <t>B2A</t>
+          <t>B2B</t>
         </is>
       </c>
       <c r="E54" s="3" t="inlineStr">
@@ -1943,12 +1930,12 @@
     <row r="55">
       <c r="A55" s="4" t="inlineStr">
         <is>
-          <t>200850</t>
+          <t>200852</t>
         </is>
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>دانيه مصطفى سالم يوسف</t>
+          <t xml:space="preserve">مجد الدين محمد الجماله </t>
         </is>
       </c>
       <c r="C55" s="4" t="inlineStr">
@@ -1970,12 +1957,12 @@
     <row r="56">
       <c r="A56" s="3" t="inlineStr">
         <is>
-          <t>200852</t>
+          <t>200858</t>
         </is>
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">مجد الدين محمد الجماله </t>
+          <t xml:space="preserve">فارس اسامه محمد فارس اسليم  </t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -1997,12 +1984,12 @@
     <row r="57">
       <c r="A57" s="4" t="inlineStr">
         <is>
-          <t>200858</t>
+          <t>200866</t>
         </is>
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">فارس اسامه محمد فارس اسليم  </t>
+          <t>ليلى مروان على شعت</t>
         </is>
       </c>
       <c r="C57" s="4" t="inlineStr">
@@ -2024,12 +2011,12 @@
     <row r="58">
       <c r="A58" s="3" t="inlineStr">
         <is>
-          <t>200866</t>
+          <t>200869</t>
         </is>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>ليلى مروان على شعت</t>
+          <t>انس الامام</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -2051,12 +2038,12 @@
     <row r="59">
       <c r="A59" s="4" t="inlineStr">
         <is>
-          <t>200869</t>
+          <t>200877</t>
         </is>
       </c>
       <c r="B59" s="4" t="inlineStr">
         <is>
-          <t>انس الامام</t>
+          <t xml:space="preserve">الاء خالد السماعيل </t>
         </is>
       </c>
       <c r="C59" s="4" t="inlineStr">
@@ -2078,12 +2065,12 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>200877</t>
+          <t>200897</t>
         </is>
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">الاء خالد السماعيل </t>
+          <t>ريناد بارى ابراهيم عثمان</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2105,12 +2092,12 @@
     <row r="61">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>200897</t>
+          <t>200904</t>
         </is>
       </c>
       <c r="B61" s="4" t="inlineStr">
         <is>
-          <t>ريناد بارى ابراهيم عثمان</t>
+          <t>سيف خالد موسى عبيد</t>
         </is>
       </c>
       <c r="C61" s="4" t="inlineStr">
@@ -2132,12 +2119,12 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>200904</t>
+          <t>200905</t>
         </is>
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>سيف خالد موسى عبيد</t>
+          <t>عبد الله بدر الدين عبد الله احمد</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -2159,12 +2146,12 @@
     <row r="63">
       <c r="A63" s="4" t="inlineStr">
         <is>
-          <t>200905</t>
+          <t>200914</t>
         </is>
       </c>
       <c r="B63" s="4" t="inlineStr">
         <is>
-          <t>عبد الله بدر الدين عبد الله احمد</t>
+          <t>زيد محمد سليم السخارنه</t>
         </is>
       </c>
       <c r="C63" s="4" t="inlineStr">
@@ -2186,12 +2173,12 @@
     <row r="64">
       <c r="A64" s="3" t="inlineStr">
         <is>
-          <t>200914</t>
+          <t>200917</t>
         </is>
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>زيد محمد سليم السخارنه</t>
+          <t>جعفر محمد الجاسم</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -2213,12 +2200,12 @@
     <row r="65">
       <c r="A65" s="4" t="inlineStr">
         <is>
-          <t>200917</t>
+          <t>200928</t>
         </is>
       </c>
       <c r="B65" s="4" t="inlineStr">
         <is>
-          <t>جعفر محمد الجاسم</t>
+          <t>المنذر بسام ابراهيم العطيوى</t>
         </is>
       </c>
       <c r="C65" s="4" t="inlineStr">
@@ -2240,12 +2227,12 @@
     <row r="66">
       <c r="A66" s="3" t="inlineStr">
         <is>
-          <t>200928</t>
+          <t>200933</t>
         </is>
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>المنذر بسام ابراهيم العطيوى</t>
+          <t xml:space="preserve">ميس عمر حسن النصيرات </t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -2267,12 +2254,12 @@
     <row r="67">
       <c r="A67" s="4" t="inlineStr">
         <is>
-          <t>200933</t>
+          <t>200938</t>
         </is>
       </c>
       <c r="B67" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ميس عمر حسن النصيرات </t>
+          <t>محمد جعفر عبده ابو رمان</t>
         </is>
       </c>
       <c r="C67" s="4" t="inlineStr">
@@ -2294,12 +2281,12 @@
     <row r="68">
       <c r="A68" s="3" t="inlineStr">
         <is>
-          <t>200938</t>
+          <t>200943</t>
         </is>
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>محمد جعفر عبده ابو رمان</t>
+          <t>محمد احيد سيدى محمد احمد</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -2321,12 +2308,12 @@
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>200943</t>
+          <t>200958</t>
         </is>
       </c>
       <c r="B69" s="4" t="inlineStr">
         <is>
-          <t>محمد احيد سيدى محمد احمد</t>
+          <t>على معاذ على عثمان</t>
         </is>
       </c>
       <c r="C69" s="4" t="inlineStr">
@@ -2348,12 +2335,12 @@
     <row r="70">
       <c r="A70" s="3" t="inlineStr">
         <is>
-          <t>200958</t>
+          <t>200968</t>
         </is>
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>على معاذ على عثمان</t>
+          <t xml:space="preserve">فيصل فهد عمر بافرج </t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -2375,12 +2362,12 @@
     <row r="71">
       <c r="A71" s="4" t="inlineStr">
         <is>
-          <t>200968</t>
+          <t>200994</t>
         </is>
       </c>
       <c r="B71" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">فيصل فهد عمر بافرج </t>
+          <t>مريم عبد الرزاق جامع</t>
         </is>
       </c>
       <c r="C71" s="4" t="inlineStr">
@@ -2402,12 +2389,12 @@
     <row r="72">
       <c r="A72" s="3" t="inlineStr">
         <is>
-          <t>200994</t>
+          <t>200997</t>
         </is>
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>مريم عبد الرزاق جامع</t>
+          <t>حلا محمود حسين العسولى</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -2429,12 +2416,12 @@
     <row r="73">
       <c r="A73" s="4" t="inlineStr">
         <is>
-          <t>200997</t>
+          <t>200999</t>
         </is>
       </c>
       <c r="B73" s="4" t="inlineStr">
         <is>
-          <t>حلا محمود حسين العسولى</t>
+          <t xml:space="preserve">خليل عاطف محمد خليل طبش </t>
         </is>
       </c>
       <c r="C73" s="4" t="inlineStr">
@@ -2456,12 +2443,12 @@
     <row r="74">
       <c r="A74" s="3" t="inlineStr">
         <is>
-          <t>200999</t>
+          <t>201013</t>
         </is>
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">خليل عاطف محمد خليل طبش </t>
+          <t>اياد محمد مؤمن ابو البرغل</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -2483,12 +2470,12 @@
     <row r="75">
       <c r="A75" s="4" t="inlineStr">
         <is>
-          <t>201013</t>
+          <t>201022</t>
         </is>
       </c>
       <c r="B75" s="4" t="inlineStr">
         <is>
-          <t>اياد محمد مؤمن ابو البرغل</t>
+          <t>محمد اسامه محمد حسن عبد الوهاب</t>
         </is>
       </c>
       <c r="C75" s="4" t="inlineStr">
@@ -2510,12 +2497,12 @@
     <row r="76">
       <c r="A76" s="3" t="inlineStr">
         <is>
-          <t>201022</t>
+          <t>201023</t>
         </is>
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>محمد اسامه محمد حسن عبد الوهاب</t>
+          <t>دانيا ناصر محمد ابو يوسف</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
@@ -2537,12 +2524,12 @@
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>201023</t>
+          <t>201026</t>
         </is>
       </c>
       <c r="B77" s="4" t="inlineStr">
         <is>
-          <t>دانيا ناصر محمد ابو يوسف</t>
+          <t>يمنى احمد عبد الله محمد</t>
         </is>
       </c>
       <c r="C77" s="4" t="inlineStr">
@@ -2564,12 +2551,12 @@
     <row r="78">
       <c r="A78" s="3" t="inlineStr">
         <is>
-          <t>201026</t>
+          <t>201051</t>
         </is>
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>يمنى احمد عبد الله محمد</t>
+          <t>رزان احمد حسن باشماخ</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -2591,12 +2578,12 @@
     <row r="79">
       <c r="A79" s="4" t="inlineStr">
         <is>
-          <t>201051</t>
+          <t>201065</t>
         </is>
       </c>
       <c r="B79" s="4" t="inlineStr">
         <is>
-          <t>رزان احمد حسن باشماخ</t>
+          <t>عباده فراس محمد النسور</t>
         </is>
       </c>
       <c r="C79" s="4" t="inlineStr">
@@ -2618,12 +2605,12 @@
     <row r="80">
       <c r="A80" s="3" t="inlineStr">
         <is>
-          <t>201065</t>
+          <t>201080</t>
         </is>
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>عباده فراس محمد النسور</t>
+          <t>زياد محمد سعد عيد رشوان</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">
@@ -2645,12 +2632,12 @@
     <row r="81">
       <c r="A81" s="4" t="inlineStr">
         <is>
-          <t>201080</t>
+          <t>201157</t>
         </is>
       </c>
       <c r="B81" s="4" t="inlineStr">
         <is>
-          <t>زياد محمد سعد عيد رشوان</t>
+          <t>حلمى عبد الغنى حلمى عبد الغنى جادو</t>
         </is>
       </c>
       <c r="C81" s="4" t="inlineStr">
@@ -2672,12 +2659,12 @@
     <row r="82">
       <c r="A82" s="3" t="inlineStr">
         <is>
-          <t>201157</t>
+          <t>201171</t>
         </is>
       </c>
       <c r="B82" s="3" t="inlineStr">
         <is>
-          <t>حلمى عبد الغنى حلمى عبد الغنى جادو</t>
+          <t>رحمه احمد محمد على خليل</t>
         </is>
       </c>
       <c r="C82" s="3" t="inlineStr">
@@ -2699,12 +2686,12 @@
     <row r="83">
       <c r="A83" s="4" t="inlineStr">
         <is>
-          <t>201171</t>
+          <t>201190</t>
         </is>
       </c>
       <c r="B83" s="4" t="inlineStr">
         <is>
-          <t>رحمه احمد محمد على خليل</t>
+          <t>مازن ضيف الله فالح عمر قنديل</t>
         </is>
       </c>
       <c r="C83" s="4" t="inlineStr">
@@ -2726,12 +2713,12 @@
     <row r="84">
       <c r="A84" s="3" t="inlineStr">
         <is>
-          <t>201190</t>
+          <t>201197</t>
         </is>
       </c>
       <c r="B84" s="3" t="inlineStr">
         <is>
-          <t>مازن ضيف الله فالح عمر قنديل</t>
+          <t xml:space="preserve">مروان حمزه ابراهيم زقوت </t>
         </is>
       </c>
       <c r="C84" s="3" t="inlineStr">
@@ -2753,12 +2740,12 @@
     <row r="85">
       <c r="A85" s="4" t="inlineStr">
         <is>
-          <t>201197</t>
+          <t>201218</t>
         </is>
       </c>
       <c r="B85" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">مروان حمزه ابراهيم زقوت </t>
+          <t>عدى بشار رياض ابراهيم</t>
         </is>
       </c>
       <c r="C85" s="4" t="inlineStr">
@@ -2780,12 +2767,12 @@
     <row r="86">
       <c r="A86" s="3" t="inlineStr">
         <is>
-          <t>201218</t>
+          <t>201237</t>
         </is>
       </c>
       <c r="B86" s="3" t="inlineStr">
         <is>
-          <t>عدى بشار رياض ابراهيم</t>
+          <t>وليد سعد وليد عابدين</t>
         </is>
       </c>
       <c r="C86" s="3" t="inlineStr">
@@ -2807,12 +2794,12 @@
     <row r="87">
       <c r="A87" s="4" t="inlineStr">
         <is>
-          <t>201237</t>
+          <t>201252</t>
         </is>
       </c>
       <c r="B87" s="4" t="inlineStr">
         <is>
-          <t>وليد سعد وليد عابدين</t>
+          <t>خزامه ابراهيم مهاوش الحماد</t>
         </is>
       </c>
       <c r="C87" s="4" t="inlineStr">
@@ -2834,12 +2821,12 @@
     <row r="88">
       <c r="A88" s="3" t="inlineStr">
         <is>
-          <t>201252</t>
+          <t>201253</t>
         </is>
       </c>
       <c r="B88" s="3" t="inlineStr">
         <is>
-          <t>خزامه ابراهيم مهاوش الحماد</t>
+          <t>الما ابراهيم مهاوش الحماد</t>
         </is>
       </c>
       <c r="C88" s="3" t="inlineStr">
@@ -2861,12 +2848,12 @@
     <row r="89">
       <c r="A89" s="4" t="inlineStr">
         <is>
-          <t>201253</t>
+          <t>201255</t>
         </is>
       </c>
       <c r="B89" s="4" t="inlineStr">
         <is>
-          <t>الما ابراهيم مهاوش الحماد</t>
+          <t>مؤمن محمود محمد الصبيحى</t>
         </is>
       </c>
       <c r="C89" s="4" t="inlineStr">
@@ -2888,12 +2875,12 @@
     <row r="90">
       <c r="A90" s="3" t="inlineStr">
         <is>
-          <t>201255</t>
+          <t>201297</t>
         </is>
       </c>
       <c r="B90" s="3" t="inlineStr">
         <is>
-          <t>مؤمن محمود محمد الصبيحى</t>
+          <t xml:space="preserve">امال منذر عبد الحميد الخرابشه </t>
         </is>
       </c>
       <c r="C90" s="3" t="inlineStr">
@@ -2915,12 +2902,12 @@
     <row r="91">
       <c r="A91" s="4" t="inlineStr">
         <is>
-          <t>201297</t>
+          <t>201328</t>
         </is>
       </c>
       <c r="B91" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">امال منذر عبد الحميد الخرابشه </t>
+          <t xml:space="preserve">اروى مفتاح محمد خليفه  </t>
         </is>
       </c>
       <c r="C91" s="4" t="inlineStr">
@@ -2942,12 +2929,12 @@
     <row r="92">
       <c r="A92" s="3" t="inlineStr">
         <is>
-          <t>201328</t>
+          <t>201337</t>
         </is>
       </c>
       <c r="B92" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">اروى مفتاح محمد خليفه  </t>
+          <t xml:space="preserve">نور حازم نعيم الصمادى  </t>
         </is>
       </c>
       <c r="C92" s="3" t="inlineStr">
@@ -2969,12 +2956,12 @@
     <row r="93">
       <c r="A93" s="4" t="inlineStr">
         <is>
-          <t>201337</t>
+          <t>201343</t>
         </is>
       </c>
       <c r="B93" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">نور حازم نعيم الصمادى  </t>
+          <t>ربى ابراهيم محمد العمرو</t>
         </is>
       </c>
       <c r="C93" s="4" t="inlineStr">
@@ -2996,12 +2983,12 @@
     <row r="94">
       <c r="A94" s="3" t="inlineStr">
         <is>
-          <t>201343</t>
+          <t>201397</t>
         </is>
       </c>
       <c r="B94" s="3" t="inlineStr">
         <is>
-          <t>ربى ابراهيم محمد العمرو</t>
+          <t xml:space="preserve">مروان عبده عبد الجليل العولقى </t>
         </is>
       </c>
       <c r="C94" s="3" t="inlineStr">
@@ -3023,12 +3010,12 @@
     <row r="95">
       <c r="A95" s="4" t="inlineStr">
         <is>
-          <t>201397</t>
+          <t>201398</t>
         </is>
       </c>
       <c r="B95" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">مروان عبده عبد الجليل العولقى </t>
+          <t xml:space="preserve">مرح وليد عبد الفتاح عزام </t>
         </is>
       </c>
       <c r="C95" s="4" t="inlineStr">
@@ -3050,12 +3037,12 @@
     <row r="96">
       <c r="A96" s="3" t="inlineStr">
         <is>
-          <t>201398</t>
+          <t>201438</t>
         </is>
       </c>
       <c r="B96" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">مرح وليد عبد الفتاح عزام </t>
+          <t>غيث معاذ محمد على</t>
         </is>
       </c>
       <c r="C96" s="3" t="inlineStr">
@@ -3077,12 +3064,12 @@
     <row r="97">
       <c r="A97" s="4" t="inlineStr">
         <is>
-          <t>201438</t>
+          <t>201465</t>
         </is>
       </c>
       <c r="B97" s="4" t="inlineStr">
         <is>
-          <t>غيث معاذ محمد على</t>
+          <t>علياء محمد بكر الكفراوى</t>
         </is>
       </c>
       <c r="C97" s="4" t="inlineStr">
@@ -3104,12 +3091,12 @@
     <row r="98">
       <c r="A98" s="3" t="inlineStr">
         <is>
-          <t>201465</t>
+          <t>201495</t>
         </is>
       </c>
       <c r="B98" s="3" t="inlineStr">
         <is>
-          <t>علياء محمد بكر الكفراوى</t>
+          <t xml:space="preserve">عبدالله خالد عبدالله عثمان  </t>
         </is>
       </c>
       <c r="C98" s="3" t="inlineStr">
@@ -3131,12 +3118,12 @@
     <row r="99">
       <c r="A99" s="4" t="inlineStr">
         <is>
-          <t>201495</t>
+          <t>201501</t>
         </is>
       </c>
       <c r="B99" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">عبدالله خالد عبدالله عثمان  </t>
+          <t>احمد حسين محمد</t>
         </is>
       </c>
       <c r="C99" s="4" t="inlineStr">
@@ -3158,12 +3145,12 @@
     <row r="100">
       <c r="A100" s="3" t="inlineStr">
         <is>
-          <t>201501</t>
+          <t>201513</t>
         </is>
       </c>
       <c r="B100" s="3" t="inlineStr">
         <is>
-          <t>احمد حسين محمد</t>
+          <t>Abdulhakim Saleh Mohamed Taha</t>
         </is>
       </c>
       <c r="C100" s="3" t="inlineStr">
@@ -3185,12 +3172,12 @@
     <row r="101">
       <c r="A101" s="4" t="inlineStr">
         <is>
-          <t>201513</t>
+          <t>201529</t>
         </is>
       </c>
       <c r="B101" s="4" t="inlineStr">
         <is>
-          <t>Abdulhakim Saleh Mohamed Taha</t>
+          <t>تذكار سليمان عيسى احمد دينار</t>
         </is>
       </c>
       <c r="C101" s="4" t="inlineStr">
@@ -3212,12 +3199,12 @@
     <row r="102">
       <c r="A102" s="3" t="inlineStr">
         <is>
-          <t>201529</t>
+          <t>201560</t>
         </is>
       </c>
       <c r="B102" s="3" t="inlineStr">
         <is>
-          <t>تذكار سليمان عيسى احمد دينار</t>
+          <t>صهيب محمد عبد الخالق طه</t>
         </is>
       </c>
       <c r="C102" s="3" t="inlineStr">
@@ -3239,12 +3226,12 @@
     <row r="103">
       <c r="A103" s="4" t="inlineStr">
         <is>
-          <t>201560</t>
+          <t>201563</t>
         </is>
       </c>
       <c r="B103" s="4" t="inlineStr">
         <is>
-          <t>صهيب محمد عبد الخالق طه</t>
+          <t>اسماء محمد ابراهيم</t>
         </is>
       </c>
       <c r="C103" s="4" t="inlineStr">
@@ -3266,12 +3253,12 @@
     <row r="104">
       <c r="A104" s="3" t="inlineStr">
         <is>
-          <t>201563</t>
+          <t>201564</t>
         </is>
       </c>
       <c r="B104" s="3" t="inlineStr">
         <is>
-          <t>اسماء محمد ابراهيم</t>
+          <t>فاطمه محمود محمد محمود</t>
         </is>
       </c>
       <c r="C104" s="3" t="inlineStr">
@@ -3293,12 +3280,12 @@
     <row r="105">
       <c r="A105" s="4" t="inlineStr">
         <is>
-          <t>201564</t>
+          <t>201572</t>
         </is>
       </c>
       <c r="B105" s="4" t="inlineStr">
         <is>
-          <t>فاطمه محمود محمد محمود</t>
+          <t>رهف عبد الرحمن سرور</t>
         </is>
       </c>
       <c r="C105" s="4" t="inlineStr">
@@ -3320,12 +3307,12 @@
     <row r="106">
       <c r="A106" s="3" t="inlineStr">
         <is>
-          <t>201572</t>
+          <t>201574</t>
         </is>
       </c>
       <c r="B106" s="3" t="inlineStr">
         <is>
-          <t>رهف عبد الرحمن سرور</t>
+          <t xml:space="preserve">مؤمل نضال عبد جون  </t>
         </is>
       </c>
       <c r="C106" s="3" t="inlineStr">
@@ -3347,12 +3334,12 @@
     <row r="107">
       <c r="A107" s="4" t="inlineStr">
         <is>
-          <t>201574</t>
+          <t>201632</t>
         </is>
       </c>
       <c r="B107" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">مؤمل نضال عبد جون  </t>
+          <t>احمد محمد مصطفى على دنيال</t>
         </is>
       </c>
       <c r="C107" s="4" t="inlineStr">
@@ -3374,12 +3361,12 @@
     <row r="108">
       <c r="A108" s="3" t="inlineStr">
         <is>
-          <t>201632</t>
+          <t>201638</t>
         </is>
       </c>
       <c r="B108" s="3" t="inlineStr">
         <is>
-          <t>احمد محمد مصطفى على دنيال</t>
+          <t>زياد محمود السيد</t>
         </is>
       </c>
       <c r="C108" s="3" t="inlineStr">
@@ -3401,12 +3388,12 @@
     <row r="109">
       <c r="A109" s="4" t="inlineStr">
         <is>
-          <t>201638</t>
+          <t>201669</t>
         </is>
       </c>
       <c r="B109" s="4" t="inlineStr">
         <is>
-          <t>زياد محمود السيد</t>
+          <t>نورهان السيد حسن محمد القزاز</t>
         </is>
       </c>
       <c r="C109" s="4" t="inlineStr">
@@ -3428,12 +3415,12 @@
     <row r="110">
       <c r="A110" s="3" t="inlineStr">
         <is>
-          <t>201669</t>
+          <t>201670</t>
         </is>
       </c>
       <c r="B110" s="3" t="inlineStr">
         <is>
-          <t>نورهان السيد حسن محمد القزاز</t>
+          <t>روان شعبان على محمد ابو هيبه</t>
         </is>
       </c>
       <c r="C110" s="3" t="inlineStr">
@@ -3455,12 +3442,12 @@
     <row r="111">
       <c r="A111" s="4" t="inlineStr">
         <is>
-          <t>201670</t>
+          <t>201682</t>
         </is>
       </c>
       <c r="B111" s="4" t="inlineStr">
         <is>
-          <t>روان شعبان على محمد ابو هيبه</t>
+          <t>خلود خالد اسماعيل عثمان صالح</t>
         </is>
       </c>
       <c r="C111" s="4" t="inlineStr">
@@ -3470,7 +3457,7 @@
       </c>
       <c r="D111" s="4" t="inlineStr">
         <is>
-          <t>B2B</t>
+          <t>B2C</t>
         </is>
       </c>
       <c r="E111" s="4" t="inlineStr">
@@ -3482,12 +3469,12 @@
     <row r="112">
       <c r="A112" s="3" t="inlineStr">
         <is>
-          <t>201682</t>
+          <t>201795</t>
         </is>
       </c>
       <c r="B112" s="3" t="inlineStr">
         <is>
-          <t>خلود خالد اسماعيل عثمان صالح</t>
+          <t xml:space="preserve">عائد احمد خليل </t>
         </is>
       </c>
       <c r="C112" s="3" t="inlineStr">
@@ -3509,12 +3496,12 @@
     <row r="113">
       <c r="A113" s="4" t="inlineStr">
         <is>
-          <t>201795</t>
+          <t>201819</t>
         </is>
       </c>
       <c r="B113" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">عائد احمد خليل </t>
+          <t xml:space="preserve">باقر على خليفة </t>
         </is>
       </c>
       <c r="C113" s="4" t="inlineStr">
@@ -3536,12 +3523,12 @@
     <row r="114">
       <c r="A114" s="3" t="inlineStr">
         <is>
-          <t>201819</t>
+          <t>201823</t>
         </is>
       </c>
       <c r="B114" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">باقر على خليفة </t>
+          <t xml:space="preserve">ابراهيم عماد عابد عابد </t>
         </is>
       </c>
       <c r="C114" s="3" t="inlineStr">
@@ -3563,12 +3550,12 @@
     <row r="115">
       <c r="A115" s="4" t="inlineStr">
         <is>
-          <t>201823</t>
+          <t>201825</t>
         </is>
       </c>
       <c r="B115" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ابراهيم عماد عابد عابد </t>
+          <t>الحمزه عماد محمد</t>
         </is>
       </c>
       <c r="C115" s="4" t="inlineStr">
@@ -3590,12 +3577,12 @@
     <row r="116">
       <c r="A116" s="3" t="inlineStr">
         <is>
-          <t>201825</t>
+          <t>201834</t>
         </is>
       </c>
       <c r="B116" s="3" t="inlineStr">
         <is>
-          <t>الحمزه عماد محمد</t>
+          <t xml:space="preserve">Mohamed Mohamed Sayed Hussien </t>
         </is>
       </c>
       <c r="C116" s="3" t="inlineStr">
@@ -3617,12 +3604,12 @@
     <row r="117">
       <c r="A117" s="4" t="inlineStr">
         <is>
-          <t>201834</t>
+          <t>201838</t>
         </is>
       </c>
       <c r="B117" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mohamed Mohamed Sayed Hussien </t>
+          <t>سائد عاصم سليمان اسماعيل الاغا</t>
         </is>
       </c>
       <c r="C117" s="4" t="inlineStr">
@@ -3644,12 +3631,12 @@
     <row r="118">
       <c r="A118" s="3" t="inlineStr">
         <is>
-          <t>201838</t>
+          <t>201840</t>
         </is>
       </c>
       <c r="B118" s="3" t="inlineStr">
         <is>
-          <t>سائد عاصم سليمان اسماعيل الاغا</t>
+          <t>يونس اسماعيل سليمان</t>
         </is>
       </c>
       <c r="C118" s="3" t="inlineStr">
@@ -3671,12 +3658,12 @@
     <row r="119">
       <c r="A119" s="4" t="inlineStr">
         <is>
-          <t>201840</t>
+          <t>201880</t>
         </is>
       </c>
       <c r="B119" s="4" t="inlineStr">
         <is>
-          <t>يونس اسماعيل سليمان</t>
+          <t>شيماء عبد الباسط عبد الصمد درويش</t>
         </is>
       </c>
       <c r="C119" s="4" t="inlineStr">
@@ -3698,12 +3685,12 @@
     <row r="120">
       <c r="A120" s="3" t="inlineStr">
         <is>
-          <t>201880</t>
+          <t>201931</t>
         </is>
       </c>
       <c r="B120" s="3" t="inlineStr">
         <is>
-          <t>شيماء عبد الباسط عبد الصمد درويش</t>
+          <t xml:space="preserve">بكر عمر محى الدين  </t>
         </is>
       </c>
       <c r="C120" s="3" t="inlineStr">
@@ -3725,12 +3712,12 @@
     <row r="121">
       <c r="A121" s="4" t="inlineStr">
         <is>
-          <t>201931</t>
+          <t>201954</t>
         </is>
       </c>
       <c r="B121" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">بكر عمر محى الدين  </t>
+          <t xml:space="preserve">احمد صباح محمد </t>
         </is>
       </c>
       <c r="C121" s="4" t="inlineStr">
@@ -3752,12 +3739,12 @@
     <row r="122">
       <c r="A122" s="3" t="inlineStr">
         <is>
-          <t>201954</t>
+          <t>201959</t>
         </is>
       </c>
       <c r="B122" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">احمد صباح محمد </t>
+          <t xml:space="preserve">صافى محمد عبد </t>
         </is>
       </c>
       <c r="C122" s="3" t="inlineStr">
@@ -3779,12 +3766,12 @@
     <row r="123">
       <c r="A123" s="4" t="inlineStr">
         <is>
-          <t>201959</t>
+          <t>201990</t>
         </is>
       </c>
       <c r="B123" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">صافى محمد عبد </t>
+          <t>زينب اسعد عبد الله المحمداوى</t>
         </is>
       </c>
       <c r="C123" s="4" t="inlineStr">
@@ -3806,12 +3793,12 @@
     <row r="124">
       <c r="A124" s="3" t="inlineStr">
         <is>
-          <t>201990</t>
+          <t>202004</t>
         </is>
       </c>
       <c r="B124" s="3" t="inlineStr">
         <is>
-          <t>زينب اسعد عبد الله المحمداوى</t>
+          <t>سلسبيل عادل عبد المعطى مطاوع موسى</t>
         </is>
       </c>
       <c r="C124" s="3" t="inlineStr">
@@ -3833,12 +3820,12 @@
     <row r="125">
       <c r="A125" s="4" t="inlineStr">
         <is>
-          <t>202004</t>
+          <t>202022</t>
         </is>
       </c>
       <c r="B125" s="4" t="inlineStr">
         <is>
-          <t>سلسبيل عادل عبد المعطى مطاوع موسى</t>
+          <t xml:space="preserve">سالى محمد حسن   </t>
         </is>
       </c>
       <c r="C125" s="4" t="inlineStr">
@@ -3860,12 +3847,12 @@
     <row r="126">
       <c r="A126" s="3" t="inlineStr">
         <is>
-          <t>202022</t>
+          <t>202028</t>
         </is>
       </c>
       <c r="B126" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">سالى محمد حسن   </t>
+          <t xml:space="preserve">حسن ضرغام كمال </t>
         </is>
       </c>
       <c r="C126" s="3" t="inlineStr">
@@ -3887,12 +3874,12 @@
     <row r="127">
       <c r="A127" s="4" t="inlineStr">
         <is>
-          <t>202028</t>
+          <t>202041</t>
         </is>
       </c>
       <c r="B127" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">حسن ضرغام كمال </t>
+          <t xml:space="preserve">محمد سعد وحيد </t>
         </is>
       </c>
       <c r="C127" s="4" t="inlineStr">
@@ -3914,12 +3901,12 @@
     <row r="128">
       <c r="A128" s="3" t="inlineStr">
         <is>
-          <t>202041</t>
+          <t>202089</t>
         </is>
       </c>
       <c r="B128" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">محمد سعد وحيد </t>
+          <t xml:space="preserve">مينا حسنين عباس </t>
         </is>
       </c>
       <c r="C128" s="3" t="inlineStr">
@@ -3941,12 +3928,12 @@
     <row r="129">
       <c r="A129" s="4" t="inlineStr">
         <is>
-          <t>202089</t>
+          <t>202162</t>
         </is>
       </c>
       <c r="B129" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">مينا حسنين عباس </t>
+          <t>محمد عاهد محمد الصرايره</t>
         </is>
       </c>
       <c r="C129" s="4" t="inlineStr">
@@ -3968,12 +3955,12 @@
     <row r="130">
       <c r="A130" s="3" t="inlineStr">
         <is>
-          <t>202162</t>
+          <t>210624</t>
         </is>
       </c>
       <c r="B130" s="3" t="inlineStr">
         <is>
-          <t>محمد عاهد محمد الصرايره</t>
+          <t>محمد سمير يونس محمد</t>
         </is>
       </c>
       <c r="C130" s="3" t="inlineStr">
@@ -3995,12 +3982,12 @@
     <row r="131">
       <c r="A131" s="4" t="inlineStr">
         <is>
-          <t>210624</t>
+          <t>210680</t>
         </is>
       </c>
       <c r="B131" s="4" t="inlineStr">
         <is>
-          <t>محمد سمير يونس محمد</t>
+          <t>مصطفى حمدان عطا احمد عبد الله</t>
         </is>
       </c>
       <c r="C131" s="4" t="inlineStr">
@@ -4022,12 +4009,12 @@
     <row r="132">
       <c r="A132" s="3" t="inlineStr">
         <is>
-          <t>210680</t>
+          <t>210728</t>
         </is>
       </c>
       <c r="B132" s="3" t="inlineStr">
         <is>
-          <t>مصطفى حمدان عطا احمد عبد الله</t>
+          <t>ندى احمد عقل على</t>
         </is>
       </c>
       <c r="C132" s="3" t="inlineStr">
@@ -4049,12 +4036,12 @@
     <row r="133">
       <c r="A133" s="4" t="inlineStr">
         <is>
-          <t>210728</t>
+          <t>210793</t>
         </is>
       </c>
       <c r="B133" s="4" t="inlineStr">
         <is>
-          <t>ندى احمد عقل على</t>
+          <t>معاذ نزال طحينه</t>
         </is>
       </c>
       <c r="C133" s="4" t="inlineStr">
@@ -4076,12 +4063,12 @@
     <row r="134">
       <c r="A134" s="3" t="inlineStr">
         <is>
-          <t>210793</t>
+          <t>210923</t>
         </is>
       </c>
       <c r="B134" s="3" t="inlineStr">
         <is>
-          <t>معاذ نزال طحينه</t>
+          <t>علاء على حسن الاسمر</t>
         </is>
       </c>
       <c r="C134" s="3" t="inlineStr">
@@ -4103,12 +4090,12 @@
     <row r="135">
       <c r="A135" s="4" t="inlineStr">
         <is>
-          <t>210923</t>
+          <t>211004</t>
         </is>
       </c>
       <c r="B135" s="4" t="inlineStr">
         <is>
-          <t>علاء على حسن الاسمر</t>
+          <t>منتصر صالح عيسى الخطيب</t>
         </is>
       </c>
       <c r="C135" s="4" t="inlineStr">
@@ -4130,12 +4117,12 @@
     <row r="136">
       <c r="A136" s="3" t="inlineStr">
         <is>
-          <t>211004</t>
+          <t>211010</t>
         </is>
       </c>
       <c r="B136" s="3" t="inlineStr">
         <is>
-          <t>منتصر صالح عيسى الخطيب</t>
+          <t>روان فيصل احمد محمد</t>
         </is>
       </c>
       <c r="C136" s="3" t="inlineStr">
@@ -4157,12 +4144,12 @@
     <row r="137">
       <c r="A137" s="4" t="inlineStr">
         <is>
-          <t>211010</t>
+          <t>211043</t>
         </is>
       </c>
       <c r="B137" s="4" t="inlineStr">
         <is>
-          <t>روان فيصل احمد محمد</t>
+          <t>حلا محمد ياسر</t>
         </is>
       </c>
       <c r="C137" s="4" t="inlineStr">
@@ -4184,12 +4171,12 @@
     <row r="138">
       <c r="A138" s="3" t="inlineStr">
         <is>
-          <t>211043</t>
+          <t>211046</t>
         </is>
       </c>
       <c r="B138" s="3" t="inlineStr">
         <is>
-          <t>حلا محمد ياسر</t>
+          <t>نوف عبد الرحمن عبد الجليل محمد</t>
         </is>
       </c>
       <c r="C138" s="3" t="inlineStr">
@@ -4211,12 +4198,12 @@
     <row r="139">
       <c r="A139" s="4" t="inlineStr">
         <is>
-          <t>211046</t>
+          <t>211079</t>
         </is>
       </c>
       <c r="B139" s="4" t="inlineStr">
         <is>
-          <t>نوف عبد الرحمن عبد الجليل محمد</t>
+          <t>حسن محمد محى الدين بابكر</t>
         </is>
       </c>
       <c r="C139" s="4" t="inlineStr">
@@ -4238,12 +4225,12 @@
     <row r="140">
       <c r="A140" s="3" t="inlineStr">
         <is>
-          <t>211079</t>
+          <t>211086</t>
         </is>
       </c>
       <c r="B140" s="3" t="inlineStr">
         <is>
-          <t>حسن محمد محى الدين بابكر</t>
+          <t xml:space="preserve">عبد القادر حافظ عبد القادر احمد </t>
         </is>
       </c>
       <c r="C140" s="3" t="inlineStr">
@@ -4265,12 +4252,12 @@
     <row r="141">
       <c r="A141" s="4" t="inlineStr">
         <is>
-          <t>211086</t>
+          <t>211092</t>
         </is>
       </c>
       <c r="B141" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">عبد القادر حافظ عبد القادر احمد </t>
+          <t>يارا اسماعيل ابراهيم درويش</t>
         </is>
       </c>
       <c r="C141" s="4" t="inlineStr">
@@ -4292,12 +4279,12 @@
     <row r="142">
       <c r="A142" s="3" t="inlineStr">
         <is>
-          <t>211092</t>
+          <t>211096</t>
         </is>
       </c>
       <c r="B142" s="3" t="inlineStr">
         <is>
-          <t>يارا اسماعيل ابراهيم درويش</t>
+          <t xml:space="preserve">محمود سامى محمود الجلال  </t>
         </is>
       </c>
       <c r="C142" s="3" t="inlineStr">
@@ -4319,12 +4306,12 @@
     <row r="143">
       <c r="A143" s="4" t="inlineStr">
         <is>
-          <t>211096</t>
+          <t>211102</t>
         </is>
       </c>
       <c r="B143" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">محمود سامى محمود الجلال  </t>
+          <t>باسل عبد المجيد مصطفى الاعمر</t>
         </is>
       </c>
       <c r="C143" s="4" t="inlineStr">
@@ -4346,12 +4333,12 @@
     <row r="144">
       <c r="A144" s="3" t="inlineStr">
         <is>
-          <t>211102</t>
+          <t>211111</t>
         </is>
       </c>
       <c r="B144" s="3" t="inlineStr">
         <is>
-          <t>باسل عبد المجيد مصطفى الاعمر</t>
+          <t>عمار عبد المهيمن الساخن</t>
         </is>
       </c>
       <c r="C144" s="3" t="inlineStr">
@@ -4373,12 +4360,12 @@
     <row r="145">
       <c r="A145" s="4" t="inlineStr">
         <is>
-          <t>211111</t>
+          <t>211118</t>
         </is>
       </c>
       <c r="B145" s="4" t="inlineStr">
         <is>
-          <t>عمار عبد المهيمن الساخن</t>
+          <t>راما سماعيل محمود فرج فريحات</t>
         </is>
       </c>
       <c r="C145" s="4" t="inlineStr">
@@ -4400,12 +4387,12 @@
     <row r="146">
       <c r="A146" s="3" t="inlineStr">
         <is>
-          <t>211118</t>
+          <t>211121</t>
         </is>
       </c>
       <c r="B146" s="3" t="inlineStr">
         <is>
-          <t>راما سماعيل محمود فرج فريحات</t>
+          <t>فراس وائل احمد سعيد</t>
         </is>
       </c>
       <c r="C146" s="3" t="inlineStr">
@@ -4427,12 +4414,12 @@
     <row r="147">
       <c r="A147" s="4" t="inlineStr">
         <is>
-          <t>211121</t>
+          <t>211131</t>
         </is>
       </c>
       <c r="B147" s="4" t="inlineStr">
         <is>
-          <t>فراس وائل احمد سعيد</t>
+          <t xml:space="preserve">ملاذ محمد مختار حاج </t>
         </is>
       </c>
       <c r="C147" s="4" t="inlineStr">
@@ -4454,12 +4441,12 @@
     <row r="148">
       <c r="A148" s="3" t="inlineStr">
         <is>
-          <t>211131</t>
+          <t>211133</t>
         </is>
       </c>
       <c r="B148" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ملاذ محمد مختار حاج </t>
+          <t>فاطمه عبد الماجد عبد العزيز عثمان</t>
         </is>
       </c>
       <c r="C148" s="3" t="inlineStr">
@@ -4481,12 +4468,12 @@
     <row r="149">
       <c r="A149" s="4" t="inlineStr">
         <is>
-          <t>211133</t>
+          <t>211137</t>
         </is>
       </c>
       <c r="B149" s="4" t="inlineStr">
         <is>
-          <t>فاطمه عبد الماجد عبد العزيز عثمان</t>
+          <t>ضرغام بشير حامد بشير</t>
         </is>
       </c>
       <c r="C149" s="4" t="inlineStr">
@@ -4508,12 +4495,12 @@
     <row r="150">
       <c r="A150" s="3" t="inlineStr">
         <is>
-          <t>211137</t>
+          <t>211146</t>
         </is>
       </c>
       <c r="B150" s="3" t="inlineStr">
         <is>
-          <t>ضرغام بشير حامد بشير</t>
+          <t xml:space="preserve">عثمان عبد الوهاب محجوب على </t>
         </is>
       </c>
       <c r="C150" s="3" t="inlineStr">
@@ -4535,12 +4522,12 @@
     <row r="151">
       <c r="A151" s="4" t="inlineStr">
         <is>
-          <t>211146</t>
+          <t>211147</t>
         </is>
       </c>
       <c r="B151" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">عثمان عبد الوهاب محجوب على </t>
+          <t>رزان محمد بله عبد الله</t>
         </is>
       </c>
       <c r="C151" s="4" t="inlineStr">
@@ -4562,12 +4549,12 @@
     <row r="152">
       <c r="A152" s="3" t="inlineStr">
         <is>
-          <t>211147</t>
+          <t>211167</t>
         </is>
       </c>
       <c r="B152" s="3" t="inlineStr">
         <is>
-          <t>رزان محمد بله عبد الله</t>
+          <t>امينه مجدى محمد مشعل</t>
         </is>
       </c>
       <c r="C152" s="3" t="inlineStr">
@@ -4589,12 +4576,12 @@
     <row r="153">
       <c r="A153" s="4" t="inlineStr">
         <is>
-          <t>211167</t>
+          <t>211169</t>
         </is>
       </c>
       <c r="B153" s="4" t="inlineStr">
         <is>
-          <t>امينه مجدى محمد مشعل</t>
+          <t>سفيان عبد الله محمد حمران</t>
         </is>
       </c>
       <c r="C153" s="4" t="inlineStr">
@@ -4616,12 +4603,12 @@
     <row r="154">
       <c r="A154" s="3" t="inlineStr">
         <is>
-          <t>211169</t>
+          <t>211174</t>
         </is>
       </c>
       <c r="B154" s="3" t="inlineStr">
         <is>
-          <t>سفيان عبد الله محمد حمران</t>
+          <t xml:space="preserve">منعمه ابراهيم محمد على </t>
         </is>
       </c>
       <c r="C154" s="3" t="inlineStr">
@@ -4643,12 +4630,12 @@
     <row r="155">
       <c r="A155" s="4" t="inlineStr">
         <is>
-          <t>211174</t>
+          <t>211175</t>
         </is>
       </c>
       <c r="B155" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">منعمه ابراهيم محمد على </t>
+          <t xml:space="preserve">احمد مرتضى محمد مضوى </t>
         </is>
       </c>
       <c r="C155" s="4" t="inlineStr">
@@ -4670,12 +4657,12 @@
     <row r="156">
       <c r="A156" s="3" t="inlineStr">
         <is>
-          <t>211175</t>
+          <t>211177</t>
         </is>
       </c>
       <c r="B156" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">احمد مرتضى محمد مضوى </t>
+          <t xml:space="preserve">اكرم محمد علاء الدين محمد </t>
         </is>
       </c>
       <c r="C156" s="3" t="inlineStr">
@@ -4697,12 +4684,12 @@
     <row r="157">
       <c r="A157" s="4" t="inlineStr">
         <is>
-          <t>211177</t>
+          <t>211189</t>
         </is>
       </c>
       <c r="B157" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">اكرم محمد علاء الدين محمد </t>
+          <t>عمر عبد العزيز الزعبي</t>
         </is>
       </c>
       <c r="C157" s="4" t="inlineStr">
@@ -4724,12 +4711,12 @@
     <row r="158">
       <c r="A158" s="3" t="inlineStr">
         <is>
-          <t>211189</t>
+          <t>211197</t>
         </is>
       </c>
       <c r="B158" s="3" t="inlineStr">
         <is>
-          <t>عمر عبد العزيز الزعبي</t>
+          <t xml:space="preserve">Nabeel Abdalgader Adam Ibrahim </t>
         </is>
       </c>
       <c r="C158" s="3" t="inlineStr">
@@ -4751,12 +4738,12 @@
     <row r="159">
       <c r="A159" s="4" t="inlineStr">
         <is>
-          <t>211197</t>
+          <t>211210</t>
         </is>
       </c>
       <c r="B159" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Nabeel Abdalgader Adam Ibrahim </t>
+          <t xml:space="preserve">صهيب على محمد الخرابشه </t>
         </is>
       </c>
       <c r="C159" s="4" t="inlineStr">
@@ -4778,12 +4765,12 @@
     <row r="160">
       <c r="A160" s="3" t="inlineStr">
         <is>
-          <t>211210</t>
+          <t>211216</t>
         </is>
       </c>
       <c r="B160" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">صهيب على محمد الخرابشه </t>
+          <t>احمد على محمد على</t>
         </is>
       </c>
       <c r="C160" s="3" t="inlineStr">
@@ -4805,12 +4792,12 @@
     <row r="161">
       <c r="A161" s="4" t="inlineStr">
         <is>
-          <t>211216</t>
+          <t>211217</t>
         </is>
       </c>
       <c r="B161" s="4" t="inlineStr">
         <is>
-          <t>احمد على محمد على</t>
+          <t xml:space="preserve">ساجد شهاب سليمان عبد الله  </t>
         </is>
       </c>
       <c r="C161" s="4" t="inlineStr">
@@ -4832,12 +4819,12 @@
     <row r="162">
       <c r="A162" s="3" t="inlineStr">
         <is>
-          <t>211217</t>
+          <t>211242</t>
         </is>
       </c>
       <c r="B162" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">ساجد شهاب سليمان عبد الله  </t>
+          <t xml:space="preserve">مجد احمد جمعه ابو جياب </t>
         </is>
       </c>
       <c r="C162" s="3" t="inlineStr">
@@ -4859,12 +4846,12 @@
     <row r="163">
       <c r="A163" s="4" t="inlineStr">
         <is>
-          <t>211242</t>
+          <t>211245</t>
         </is>
       </c>
       <c r="B163" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">مجد احمد جمعه ابو جياب </t>
+          <t>زهره حامد سعد الله عبد الله</t>
         </is>
       </c>
       <c r="C163" s="4" t="inlineStr">
@@ -4886,12 +4873,12 @@
     <row r="164">
       <c r="A164" s="3" t="inlineStr">
         <is>
-          <t>211245</t>
+          <t>211246</t>
         </is>
       </c>
       <c r="B164" s="3" t="inlineStr">
         <is>
-          <t>زهره حامد سعد الله عبد الله</t>
+          <t>عبد الرحمن شحاده حسين طرخان</t>
         </is>
       </c>
       <c r="C164" s="3" t="inlineStr">
@@ -4913,12 +4900,12 @@
     <row r="165">
       <c r="A165" s="4" t="inlineStr">
         <is>
-          <t>211246</t>
+          <t>211741</t>
         </is>
       </c>
       <c r="B165" s="4" t="inlineStr">
         <is>
-          <t>عبد الرحمن شحاده حسين طرخان</t>
+          <t xml:space="preserve">احمد منار احمد العوينى  </t>
         </is>
       </c>
       <c r="C165" s="4" t="inlineStr">
@@ -4940,12 +4927,12 @@
     <row r="166">
       <c r="A166" s="3" t="inlineStr">
         <is>
-          <t>211741</t>
+          <t>201007</t>
         </is>
       </c>
       <c r="B166" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">احمد منار احمد العوينى  </t>
+          <t>اسامه خالد محسن المطار</t>
         </is>
       </c>
       <c r="C166" s="3" t="inlineStr">
@@ -4955,7 +4942,7 @@
       </c>
       <c r="D166" s="3" t="inlineStr">
         <is>
-          <t>B2C</t>
+          <t>B2D</t>
         </is>
       </c>
       <c r="E166" s="3" t="inlineStr">
@@ -4967,12 +4954,12 @@
     <row r="167">
       <c r="A167" s="4" t="inlineStr">
         <is>
-          <t>201007</t>
+          <t>211232</t>
         </is>
       </c>
       <c r="B167" s="4" t="inlineStr">
         <is>
-          <t>اسامه خالد محسن المطار</t>
+          <t>دانه جاسر محمد سعيد مسعود</t>
         </is>
       </c>
       <c r="C167" s="4" t="inlineStr">
@@ -4994,12 +4981,12 @@
     <row r="168">
       <c r="A168" s="3" t="inlineStr">
         <is>
-          <t>211232</t>
+          <t>211251</t>
         </is>
       </c>
       <c r="B168" s="3" t="inlineStr">
         <is>
-          <t>دانه جاسر محمد سعيد مسعود</t>
+          <t>انوار يوسف موسى الزعبى</t>
         </is>
       </c>
       <c r="C168" s="3" t="inlineStr">
@@ -5021,12 +5008,12 @@
     <row r="169">
       <c r="A169" s="4" t="inlineStr">
         <is>
-          <t>211251</t>
+          <t>211262</t>
         </is>
       </c>
       <c r="B169" s="4" t="inlineStr">
         <is>
-          <t>انوار يوسف موسى الزعبى</t>
+          <t>رغد ابراهيم محمد ابو طير</t>
         </is>
       </c>
       <c r="C169" s="4" t="inlineStr">
@@ -5048,12 +5035,12 @@
     <row r="170">
       <c r="A170" s="3" t="inlineStr">
         <is>
-          <t>211262</t>
+          <t>211263</t>
         </is>
       </c>
       <c r="B170" s="3" t="inlineStr">
         <is>
-          <t>رغد ابراهيم محمد ابو طير</t>
+          <t xml:space="preserve">عمر ابراهيم محمد الغنيمات </t>
         </is>
       </c>
       <c r="C170" s="3" t="inlineStr">
@@ -5075,12 +5062,12 @@
     <row r="171">
       <c r="A171" s="4" t="inlineStr">
         <is>
-          <t>211263</t>
+          <t>211267</t>
         </is>
       </c>
       <c r="B171" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">عمر ابراهيم محمد الغنيمات </t>
+          <t>قيس اسامه عبد الله هياجنه</t>
         </is>
       </c>
       <c r="C171" s="4" t="inlineStr">
@@ -5102,12 +5089,12 @@
     <row r="172">
       <c r="A172" s="3" t="inlineStr">
         <is>
-          <t>211267</t>
+          <t>211276</t>
         </is>
       </c>
       <c r="B172" s="3" t="inlineStr">
         <is>
-          <t>قيس اسامه عبد الله هياجنه</t>
+          <t>كمال وحيد محمد كمال عناتى</t>
         </is>
       </c>
       <c r="C172" s="3" t="inlineStr">
@@ -5129,12 +5116,12 @@
     <row r="173">
       <c r="A173" s="4" t="inlineStr">
         <is>
-          <t>211276</t>
+          <t>211286</t>
         </is>
       </c>
       <c r="B173" s="4" t="inlineStr">
         <is>
-          <t>كمال وحيد محمد كمال عناتى</t>
+          <t>اياد نبيل صادق طل</t>
         </is>
       </c>
       <c r="C173" s="4" t="inlineStr">
@@ -5156,12 +5143,12 @@
     <row r="174">
       <c r="A174" s="3" t="inlineStr">
         <is>
-          <t>211286</t>
+          <t>211288</t>
         </is>
       </c>
       <c r="B174" s="3" t="inlineStr">
         <is>
-          <t>اياد نبيل صادق طل</t>
+          <t>Ibrahim Taha Salama Helles</t>
         </is>
       </c>
       <c r="C174" s="3" t="inlineStr">
@@ -5183,12 +5170,12 @@
     <row r="175">
       <c r="A175" s="4" t="inlineStr">
         <is>
-          <t>211288</t>
+          <t>211295</t>
         </is>
       </c>
       <c r="B175" s="4" t="inlineStr">
         <is>
-          <t>Ibrahim Taha Salama Helles</t>
+          <t>هبه عبد الحميد عبد الله محمد</t>
         </is>
       </c>
       <c r="C175" s="4" t="inlineStr">
@@ -5210,12 +5197,12 @@
     <row r="176">
       <c r="A176" s="3" t="inlineStr">
         <is>
-          <t>211295</t>
+          <t>211298</t>
         </is>
       </c>
       <c r="B176" s="3" t="inlineStr">
         <is>
-          <t>هبه عبد الحميد عبد الله محمد</t>
+          <t>احمد عدنان محمود الخالد</t>
         </is>
       </c>
       <c r="C176" s="3" t="inlineStr">
@@ -5237,12 +5224,12 @@
     <row r="177">
       <c r="A177" s="4" t="inlineStr">
         <is>
-          <t>211298</t>
+          <t>211299</t>
         </is>
       </c>
       <c r="B177" s="4" t="inlineStr">
         <is>
-          <t>احمد عدنان محمود الخالد</t>
+          <t>محمد منير راضى خرفان</t>
         </is>
       </c>
       <c r="C177" s="4" t="inlineStr">
@@ -5264,12 +5251,12 @@
     <row r="178">
       <c r="A178" s="3" t="inlineStr">
         <is>
-          <t>211299</t>
+          <t>211311</t>
         </is>
       </c>
       <c r="B178" s="3" t="inlineStr">
         <is>
-          <t>محمد منير راضى خرفان</t>
+          <t>سولارا حسن صلاح الدين محمد</t>
         </is>
       </c>
       <c r="C178" s="3" t="inlineStr">
@@ -5291,12 +5278,12 @@
     <row r="179">
       <c r="A179" s="4" t="inlineStr">
         <is>
-          <t>211311</t>
+          <t>211348</t>
         </is>
       </c>
       <c r="B179" s="4" t="inlineStr">
         <is>
-          <t>سولارا حسن صلاح الدين محمد</t>
+          <t>محمد السيد عبد المنعم الغباشى</t>
         </is>
       </c>
       <c r="C179" s="4" t="inlineStr">
@@ -5318,12 +5305,12 @@
     <row r="180">
       <c r="A180" s="3" t="inlineStr">
         <is>
-          <t>211348</t>
+          <t>211399</t>
         </is>
       </c>
       <c r="B180" s="3" t="inlineStr">
         <is>
-          <t>محمد السيد عبد المنعم الغباشى</t>
+          <t>بسنت علاء الدين احمد محمد مرزوق</t>
         </is>
       </c>
       <c r="C180" s="3" t="inlineStr">
@@ -5345,12 +5332,12 @@
     <row r="181">
       <c r="A181" s="4" t="inlineStr">
         <is>
-          <t>211399</t>
+          <t>211415</t>
         </is>
       </c>
       <c r="B181" s="4" t="inlineStr">
         <is>
-          <t>بسنت علاء الدين احمد محمد مرزوق</t>
+          <t>محمد هشام محمد عبد الوهاب</t>
         </is>
       </c>
       <c r="C181" s="4" t="inlineStr">
@@ -5372,12 +5359,12 @@
     <row r="182">
       <c r="A182" s="3" t="inlineStr">
         <is>
-          <t>211415</t>
+          <t>211451</t>
         </is>
       </c>
       <c r="B182" s="3" t="inlineStr">
         <is>
-          <t>محمد هشام محمد عبد الوهاب</t>
+          <t>كارين ماجد شرقاوى يعقوب خليل</t>
         </is>
       </c>
       <c r="C182" s="3" t="inlineStr">
@@ -5399,12 +5386,12 @@
     <row r="183">
       <c r="A183" s="4" t="inlineStr">
         <is>
-          <t>211451</t>
+          <t>211457</t>
         </is>
       </c>
       <c r="B183" s="4" t="inlineStr">
         <is>
-          <t>كارين ماجد شرقاوى يعقوب خليل</t>
+          <t>جودى محمد احمد شديد</t>
         </is>
       </c>
       <c r="C183" s="4" t="inlineStr">
@@ -5426,12 +5413,12 @@
     <row r="184">
       <c r="A184" s="3" t="inlineStr">
         <is>
-          <t>211457</t>
+          <t>211486</t>
         </is>
       </c>
       <c r="B184" s="3" t="inlineStr">
         <is>
-          <t>جودى محمد احمد شديد</t>
+          <t>ادهم اشرف محمد رجائى عبد الحافظ شعبان</t>
         </is>
       </c>
       <c r="C184" s="3" t="inlineStr">
@@ -5453,12 +5440,12 @@
     <row r="185">
       <c r="A185" s="4" t="inlineStr">
         <is>
-          <t>211486</t>
+          <t>211539</t>
         </is>
       </c>
       <c r="B185" s="4" t="inlineStr">
         <is>
-          <t>ادهم اشرف محمد رجائى عبد الحافظ شعبان</t>
+          <t>عمرو هانى صالح امين حسين الصفتى</t>
         </is>
       </c>
       <c r="C185" s="4" t="inlineStr">
@@ -5480,12 +5467,12 @@
     <row r="186">
       <c r="A186" s="3" t="inlineStr">
         <is>
-          <t>211539</t>
+          <t>211553</t>
         </is>
       </c>
       <c r="B186" s="3" t="inlineStr">
         <is>
-          <t>عمرو هانى صالح امين حسين الصفتى</t>
+          <t>ريم السباعى زياد سليمان</t>
         </is>
       </c>
       <c r="C186" s="3" t="inlineStr">
@@ -5507,12 +5494,12 @@
     <row r="187">
       <c r="A187" s="4" t="inlineStr">
         <is>
-          <t>211553</t>
+          <t>211559</t>
         </is>
       </c>
       <c r="B187" s="4" t="inlineStr">
         <is>
-          <t>ريم السباعى زياد سليمان</t>
+          <t>رقيه صفوان محمد تيسير خضير</t>
         </is>
       </c>
       <c r="C187" s="4" t="inlineStr">
@@ -5534,12 +5521,12 @@
     <row r="188">
       <c r="A188" s="3" t="inlineStr">
         <is>
-          <t>211559</t>
+          <t>211560</t>
         </is>
       </c>
       <c r="B188" s="3" t="inlineStr">
         <is>
-          <t>رقيه صفوان محمد تيسير خضير</t>
+          <t>عمار ياسر الصادق محمد</t>
         </is>
       </c>
       <c r="C188" s="3" t="inlineStr">
@@ -5561,12 +5548,12 @@
     <row r="189">
       <c r="A189" s="4" t="inlineStr">
         <is>
-          <t>211560</t>
+          <t>211575</t>
         </is>
       </c>
       <c r="B189" s="4" t="inlineStr">
         <is>
-          <t>عمار ياسر الصادق محمد</t>
+          <t>ايلاف الصادق عبد الملك ابراهيم</t>
         </is>
       </c>
       <c r="C189" s="4" t="inlineStr">
@@ -5588,12 +5575,12 @@
     <row r="190">
       <c r="A190" s="3" t="inlineStr">
         <is>
-          <t>211575</t>
+          <t>211579</t>
         </is>
       </c>
       <c r="B190" s="3" t="inlineStr">
         <is>
-          <t>ايلاف الصادق عبد الملك ابراهيم</t>
+          <t>ابراهيم معتصم ابراهيم الشيخ محمد</t>
         </is>
       </c>
       <c r="C190" s="3" t="inlineStr">
@@ -5615,12 +5602,12 @@
     <row r="191">
       <c r="A191" s="4" t="inlineStr">
         <is>
-          <t>211579</t>
+          <t>211590</t>
         </is>
       </c>
       <c r="B191" s="4" t="inlineStr">
         <is>
-          <t>ابراهيم معتصم ابراهيم الشيخ محمد</t>
+          <t xml:space="preserve">عماد عبد الكريم كامل شبير </t>
         </is>
       </c>
       <c r="C191" s="4" t="inlineStr">
@@ -5642,12 +5629,12 @@
     <row r="192">
       <c r="A192" s="3" t="inlineStr">
         <is>
-          <t>211590</t>
+          <t>211598</t>
         </is>
       </c>
       <c r="B192" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">عماد عبد الكريم كامل شبير </t>
+          <t>اسحاق محمد على قاسم الصلولى</t>
         </is>
       </c>
       <c r="C192" s="3" t="inlineStr">
@@ -5669,12 +5656,12 @@
     <row r="193">
       <c r="A193" s="4" t="inlineStr">
         <is>
-          <t>211598</t>
+          <t>211603</t>
         </is>
       </c>
       <c r="B193" s="4" t="inlineStr">
         <is>
-          <t>اسحاق محمد على قاسم الصلولى</t>
+          <t>ريم رائد عبد الرحمن ابو جاسر</t>
         </is>
       </c>
       <c r="C193" s="4" t="inlineStr">
@@ -5696,12 +5683,12 @@
     <row r="194">
       <c r="A194" s="3" t="inlineStr">
         <is>
-          <t>211603</t>
+          <t>211617</t>
         </is>
       </c>
       <c r="B194" s="3" t="inlineStr">
         <is>
-          <t>ريم رائد عبد الرحمن ابو جاسر</t>
+          <t>عادل عبد السلام احمد العبادى</t>
         </is>
       </c>
       <c r="C194" s="3" t="inlineStr">
@@ -5723,12 +5710,12 @@
     <row r="195">
       <c r="A195" s="4" t="inlineStr">
         <is>
-          <t>211617</t>
+          <t>211619</t>
         </is>
       </c>
       <c r="B195" s="4" t="inlineStr">
         <is>
-          <t>عادل عبد السلام احمد العبادى</t>
+          <t>معاذ سامر عبد العزيز دردس</t>
         </is>
       </c>
       <c r="C195" s="4" t="inlineStr">
@@ -5750,12 +5737,12 @@
     <row r="196">
       <c r="A196" s="3" t="inlineStr">
         <is>
-          <t>211619</t>
+          <t>211621</t>
         </is>
       </c>
       <c r="B196" s="3" t="inlineStr">
         <is>
-          <t>معاذ سامر عبد العزيز دردس</t>
+          <t>عثمان محمد نادر كامل</t>
         </is>
       </c>
       <c r="C196" s="3" t="inlineStr">
@@ -5777,12 +5764,12 @@
     <row r="197">
       <c r="A197" s="4" t="inlineStr">
         <is>
-          <t>211621</t>
+          <t>211623</t>
         </is>
       </c>
       <c r="B197" s="4" t="inlineStr">
         <is>
-          <t>عثمان محمد نادر كامل</t>
+          <t>يحيى عز العرب احمد العزه</t>
         </is>
       </c>
       <c r="C197" s="4" t="inlineStr">
@@ -5804,12 +5791,12 @@
     <row r="198">
       <c r="A198" s="3" t="inlineStr">
         <is>
-          <t>211623</t>
+          <t>211631</t>
         </is>
       </c>
       <c r="B198" s="3" t="inlineStr">
         <is>
-          <t>يحيى عز العرب احمد العزه</t>
+          <t>فرح احمد عبد الهادى الزعاتره</t>
         </is>
       </c>
       <c r="C198" s="3" t="inlineStr">
@@ -5831,12 +5818,12 @@
     <row r="199">
       <c r="A199" s="4" t="inlineStr">
         <is>
-          <t>211631</t>
+          <t>211635</t>
         </is>
       </c>
       <c r="B199" s="4" t="inlineStr">
         <is>
-          <t>فرح احمد عبد الهادى الزعاتره</t>
+          <t xml:space="preserve">Ichraka Mahamat Oumar </t>
         </is>
       </c>
       <c r="C199" s="4" t="inlineStr">
@@ -5858,12 +5845,12 @@
     <row r="200">
       <c r="A200" s="3" t="inlineStr">
         <is>
-          <t>211635</t>
+          <t>211637</t>
         </is>
       </c>
       <c r="B200" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ichraka Mahamat Oumar </t>
+          <t>مؤيد جميل راسم الريماوى</t>
         </is>
       </c>
       <c r="C200" s="3" t="inlineStr">
@@ -5885,12 +5872,12 @@
     <row r="201">
       <c r="A201" s="4" t="inlineStr">
         <is>
-          <t>211637</t>
+          <t>211643</t>
         </is>
       </c>
       <c r="B201" s="4" t="inlineStr">
         <is>
-          <t>مؤيد جميل راسم الريماوى</t>
+          <t>Omar A H Daraghmeh</t>
         </is>
       </c>
       <c r="C201" s="4" t="inlineStr">
@@ -5912,12 +5899,12 @@
     <row r="202">
       <c r="A202" s="3" t="inlineStr">
         <is>
-          <t>211643</t>
+          <t>211648</t>
         </is>
       </c>
       <c r="B202" s="3" t="inlineStr">
         <is>
-          <t>Omar A H Daraghmeh</t>
+          <t xml:space="preserve">عبد الرحمن خالد سعيد السعدى  </t>
         </is>
       </c>
       <c r="C202" s="3" t="inlineStr">
@@ -5939,12 +5926,12 @@
     <row r="203">
       <c r="A203" s="4" t="inlineStr">
         <is>
-          <t>211648</t>
+          <t>211655</t>
         </is>
       </c>
       <c r="B203" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">عبد الرحمن خالد سعيد السعدى  </t>
+          <t xml:space="preserve">هاشم عبد الاله محمد عبد الحسن الشعبه  </t>
         </is>
       </c>
       <c r="C203" s="4" t="inlineStr">
@@ -5966,12 +5953,12 @@
     <row r="204">
       <c r="A204" s="3" t="inlineStr">
         <is>
-          <t>211655</t>
+          <t>211662</t>
         </is>
       </c>
       <c r="B204" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">هاشم عبد الاله محمد عبد الحسن الشعبه  </t>
+          <t>غاده بنت جابر بن محمد طوطيه</t>
         </is>
       </c>
       <c r="C204" s="3" t="inlineStr">
@@ -5993,12 +5980,12 @@
     <row r="205">
       <c r="A205" s="4" t="inlineStr">
         <is>
-          <t>211662</t>
+          <t>211663</t>
         </is>
       </c>
       <c r="B205" s="4" t="inlineStr">
         <is>
-          <t>غاده بنت جابر بن محمد طوطيه</t>
+          <t>ايمن احمد على عبده</t>
         </is>
       </c>
       <c r="C205" s="4" t="inlineStr">
@@ -6020,12 +6007,12 @@
     <row r="206">
       <c r="A206" s="3" t="inlineStr">
         <is>
-          <t>211663</t>
+          <t>211670</t>
         </is>
       </c>
       <c r="B206" s="3" t="inlineStr">
         <is>
-          <t>ايمن احمد على عبده</t>
+          <t>اسامه اديب على عبده الشامى</t>
         </is>
       </c>
       <c r="C206" s="3" t="inlineStr">
@@ -6047,12 +6034,12 @@
     <row r="207">
       <c r="A207" s="4" t="inlineStr">
         <is>
-          <t>211670</t>
+          <t>211672</t>
         </is>
       </c>
       <c r="B207" s="4" t="inlineStr">
         <is>
-          <t>اسامه اديب على عبده الشامى</t>
+          <t xml:space="preserve">محمد خالد محمد ابو عرار  </t>
         </is>
       </c>
       <c r="C207" s="4" t="inlineStr">
@@ -6074,12 +6061,12 @@
     <row r="208">
       <c r="A208" s="3" t="inlineStr">
         <is>
-          <t>211672</t>
+          <t>211680</t>
         </is>
       </c>
       <c r="B208" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">محمد خالد محمد ابو عرار  </t>
+          <t>لمى طلال محمد البدور</t>
         </is>
       </c>
       <c r="C208" s="3" t="inlineStr">
@@ -6101,12 +6088,12 @@
     <row r="209">
       <c r="A209" s="4" t="inlineStr">
         <is>
-          <t>211680</t>
+          <t>211687</t>
         </is>
       </c>
       <c r="B209" s="4" t="inlineStr">
         <is>
-          <t>لمى طلال محمد البدور</t>
+          <t>خيران سلطان على الحيجنه</t>
         </is>
       </c>
       <c r="C209" s="4" t="inlineStr">
@@ -6128,12 +6115,12 @@
     <row r="210">
       <c r="A210" s="3" t="inlineStr">
         <is>
-          <t>211687</t>
+          <t>211690</t>
         </is>
       </c>
       <c r="B210" s="3" t="inlineStr">
         <is>
-          <t>خيران سلطان على الحيجنه</t>
+          <t>Younes Zouhair Almbarak</t>
         </is>
       </c>
       <c r="C210" s="3" t="inlineStr">
@@ -6155,12 +6142,12 @@
     <row r="211">
       <c r="A211" s="4" t="inlineStr">
         <is>
-          <t>211690</t>
+          <t>211697</t>
         </is>
       </c>
       <c r="B211" s="4" t="inlineStr">
         <is>
-          <t>Younes Zouhair Almbarak</t>
+          <t>فاطمه الهادى ابراهيم احمد</t>
         </is>
       </c>
       <c r="C211" s="4" t="inlineStr">
@@ -6182,12 +6169,12 @@
     <row r="212">
       <c r="A212" s="3" t="inlineStr">
         <is>
-          <t>211697</t>
+          <t>211699</t>
         </is>
       </c>
       <c r="B212" s="3" t="inlineStr">
         <is>
-          <t>فاطمه الهادى ابراهيم احمد</t>
+          <t xml:space="preserve">رهف عادل على محمد احمد   </t>
         </is>
       </c>
       <c r="C212" s="3" t="inlineStr">
@@ -6209,12 +6196,12 @@
     <row r="213">
       <c r="A213" s="4" t="inlineStr">
         <is>
-          <t>211699</t>
+          <t>211710</t>
         </is>
       </c>
       <c r="B213" s="4" t="inlineStr">
         <is>
-          <t xml:space="preserve">رهف عادل على محمد احمد   </t>
+          <t>جنات فايز عزمى شماس</t>
         </is>
       </c>
       <c r="C213" s="4" t="inlineStr">
@@ -6236,12 +6223,12 @@
     <row r="214">
       <c r="A214" s="3" t="inlineStr">
         <is>
-          <t>211710</t>
+          <t>211711</t>
         </is>
       </c>
       <c r="B214" s="3" t="inlineStr">
         <is>
-          <t>جنات فايز عزمى شماس</t>
+          <t>احمد عبد الله سالم الحويان</t>
         </is>
       </c>
       <c r="C214" s="3" t="inlineStr">
@@ -6263,12 +6250,12 @@
     <row r="215">
       <c r="A215" s="4" t="inlineStr">
         <is>
-          <t>211711</t>
+          <t>211713</t>
         </is>
       </c>
       <c r="B215" s="4" t="inlineStr">
         <is>
-          <t>احمد عبد الله سالم الحويان</t>
+          <t>صفاء محمود عبد الرحيم الامين</t>
         </is>
       </c>
       <c r="C215" s="4" t="inlineStr">
@@ -6290,12 +6277,12 @@
     <row r="216">
       <c r="A216" s="3" t="inlineStr">
         <is>
-          <t>211713</t>
+          <t>211720</t>
         </is>
       </c>
       <c r="B216" s="3" t="inlineStr">
         <is>
-          <t>صفاء محمود عبد الرحيم الامين</t>
+          <t>ساره محمد احمد البيروتى</t>
         </is>
       </c>
       <c r="C216" s="3" t="inlineStr">
@@ -6317,12 +6304,12 @@
     <row r="217">
       <c r="A217" s="4" t="inlineStr">
         <is>
-          <t>211720</t>
+          <t>211723</t>
         </is>
       </c>
       <c r="B217" s="4" t="inlineStr">
         <is>
-          <t>ساره محمد احمد البيروتى</t>
+          <t>احمد حسن خليفه التليسى</t>
         </is>
       </c>
       <c r="C217" s="4" t="inlineStr">
@@ -6344,12 +6331,12 @@
     <row r="218">
       <c r="A218" s="3" t="inlineStr">
         <is>
-          <t>211723</t>
+          <t>211725</t>
         </is>
       </c>
       <c r="B218" s="3" t="inlineStr">
         <is>
-          <t>احمد حسن خليفه التليسى</t>
+          <t>زينب رفعت محمد عبد القيوم</t>
         </is>
       </c>
       <c r="C218" s="3" t="inlineStr">
@@ -6371,12 +6358,12 @@
     <row r="219">
       <c r="A219" s="4" t="inlineStr">
         <is>
-          <t>211725</t>
+          <t>211728</t>
         </is>
       </c>
       <c r="B219" s="4" t="inlineStr">
         <is>
-          <t>زينب رفعت محمد عبد القيوم</t>
+          <t xml:space="preserve">اياد احمد محمد ابو درويش </t>
         </is>
       </c>
       <c r="C219" s="4" t="inlineStr">
@@ -6398,12 +6385,12 @@
     <row r="220">
       <c r="A220" s="3" t="inlineStr">
         <is>
-          <t>211728</t>
+          <t>211732</t>
         </is>
       </c>
       <c r="B220" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">اياد احمد محمد ابو درويش </t>
+          <t>محمد يامن فراس الامام</t>
         </is>
       </c>
       <c r="C220" s="3" t="inlineStr">
@@ -6425,12 +6412,12 @@
     <row r="221">
       <c r="A221" s="4" t="inlineStr">
         <is>
-          <t>211732</t>
+          <t>211735</t>
         </is>
       </c>
       <c r="B221" s="4" t="inlineStr">
         <is>
-          <t>محمد يامن فراس الامام</t>
+          <t xml:space="preserve">عبد الله عواد رفعت ابو زيد   </t>
         </is>
       </c>
       <c r="C221" s="4" t="inlineStr">
@@ -6452,12 +6439,12 @@
     <row r="222">
       <c r="A222" s="3" t="inlineStr">
         <is>
-          <t>211735</t>
+          <t>190540</t>
         </is>
       </c>
       <c r="B222" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">عبد الله عواد رفعت ابو زيد   </t>
+          <t>ليان بنت خالد بن سعد المقذلى</t>
         </is>
       </c>
       <c r="C222" s="3" t="inlineStr">
@@ -6467,7 +6454,7 @@
       </c>
       <c r="D222" s="3" t="inlineStr">
         <is>
-          <t>B2D</t>
+          <t>B2E</t>
         </is>
       </c>
       <c r="E222" s="3" t="inlineStr">
@@ -9501,6 +9488,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>